<commit_message>
txt toegevoegd voor makkelijker edit
</commit_message>
<xml_diff>
--- a/namenlijst.xlsx
+++ b/namenlijst.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t xml:space="preserve">#Zet jezelf ff op deze lijst als je meegaat.</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nee</t>
   </si>
 </sst>
 </file>
@@ -55,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -76,12 +83,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -89,6 +98,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -138,14 +148,16 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -153,11 +165,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -169,7 +177,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Accent 2" xfId="20"/>
+    <cellStyle name="Accent 2 1" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -179,16 +187,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="4" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="2" width="11.52"/>
   </cols>
@@ -207,10 +215,10 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -225,10 +233,21 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>